<commit_message>
Moest opniew clonen en shit
Urenregistratie geadd, maar shit ging fout ofzo dus moest opnieuw clonen
en voor zekerheid mijn eigen sripts herplakken enzo.
</commit_message>
<xml_diff>
--- a/Urenregistratie/Urenregistratie.xlsx
+++ b/Urenregistratie/Urenregistratie.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="34">
   <si>
     <t>Maandag</t>
   </si>
@@ -147,12 +147,15 @@
   <si>
     <t>Overuren Over</t>
   </si>
+  <si>
+    <t>Gemiddeld:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +248,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,8 +341,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="48">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -947,12 +963,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="mediumDashed">
+        <color auto="1"/>
+      </left>
+      <right style="mediumDashed">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1019,6 +1050,8 @@
     <xf numFmtId="9" fontId="10" fillId="13" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="12" fillId="15" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -2593,8 +2626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="C82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M91" sqref="M91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2616,7 +2649,7 @@
       </c>
       <c r="B2" s="17">
         <f>SUM(Totaal_Uren_in_week)</f>
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E2" s="51" t="s">
         <v>29</v>
@@ -2654,7 +2687,7 @@
       </c>
       <c r="B4" s="13">
         <f>SUM(Official_Uren_Zinedine)</f>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E4" s="55" t="s">
         <v>6</v>
@@ -2664,7 +2697,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" s="56">
         <f>SUM(B6-G4)</f>
@@ -2677,14 +2710,14 @@
       </c>
       <c r="B5" s="7">
         <f>SUM(B2)-SUM(B4)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" s="57" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="46">
         <f>SUM((B8+G5)/B2)</f>
-        <v>0.8</v>
+        <v>0.88461538461538458</v>
       </c>
       <c r="G5" s="49">
         <v>0</v>
@@ -2700,7 +2733,7 @@
       </c>
       <c r="B6" s="15">
         <f>SUM(Totaal_Overuren_Zinedine)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6" s="57" t="s">
         <v>8</v>
@@ -2743,7 +2776,7 @@
       </c>
       <c r="B8" s="13">
         <f>SUM(Official_Uren_Harold)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E8" s="61" t="s">
         <v>10</v>
@@ -2771,7 +2804,7 @@
       </c>
       <c r="F9" s="45">
         <f>SUM((B20+G9)/B2)</f>
-        <v>0.8</v>
+        <v>0.73076923076923073</v>
       </c>
       <c r="G9" s="48">
         <v>1</v>
@@ -2830,14 +2863,14 @@
       </c>
       <c r="B12" s="13">
         <f>SUM(Official_Uren_Sven)</f>
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E12" s="57" t="s">
         <v>26</v>
       </c>
       <c r="F12" s="46">
         <f>SUM((B32+G12)/B2)</f>
-        <v>0.93333333333333335</v>
+        <v>0.84615384615384615</v>
       </c>
       <c r="G12" s="49">
         <v>0</v>
@@ -2890,14 +2923,29 @@
       </c>
       <c r="H14" s="65">
         <f>SUM(B42-G14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="11"/>
+      <c r="E15" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="67">
+        <f>AVERAGE(F4,F5,F6,F7,F9,F10,F11,F12,F13,F14)</f>
+        <v>0.94615384615384601</v>
+      </c>
+      <c r="G15" s="66">
+        <f>AVERAGE(G4,G5,G6,G7,G9,G10,G11,G12,G13,G14)</f>
+        <v>0.3</v>
+      </c>
+      <c r="H15" s="66">
+        <f>AVERAGE(H4,H5,H6,H7,H9,H10,H11,H12,H13,H14)</f>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
@@ -2905,7 +2953,7 @@
       </c>
       <c r="B16" s="13">
         <f>SUM(Official_Uren_Mack)</f>
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2938,7 +2986,7 @@
       </c>
       <c r="B20" s="13">
         <f>SUM(Official_Uren_Michiel)</f>
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2947,7 +2995,7 @@
       </c>
       <c r="B21" s="7">
         <f>SUM(B2)-SUM(B20)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2971,7 +3019,7 @@
       </c>
       <c r="B24" s="13">
         <f>SUM(Official_Uren_Anthony)</f>
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3004,7 +3052,7 @@
       </c>
       <c r="B28" s="13">
         <f>SUM(Official_Uren_Kevin)</f>
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3037,7 +3085,7 @@
       </c>
       <c r="B32" s="13">
         <f>SUM(Official_Uren_Killian)</f>
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3046,7 +3094,7 @@
       </c>
       <c r="B33" s="7">
         <f>SUM(B2)-SUM(B32)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3070,7 +3118,7 @@
       </c>
       <c r="B36" s="13">
         <f>SUM(Official_Uren_Roos)</f>
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3103,7 +3151,7 @@
       </c>
       <c r="B40" s="13">
         <f>SUM(Official_Uren_Carlo)</f>
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3121,7 +3169,7 @@
       </c>
       <c r="B42" s="8">
         <f>SUM(Totaal_Overuren_Carlo)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.45">
@@ -4110,7 +4158,7 @@
         <v>20</v>
       </c>
       <c r="K70" s="30">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="4:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4145,7 +4193,7 @@
         <v>2</v>
       </c>
       <c r="F72" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G72" s="1">
         <v>3</v>
@@ -4158,7 +4206,7 @@
       </c>
       <c r="J72" s="24">
         <f t="shared" ref="J72:J79" si="4">SUM(E72+F72+G72+H72+I72)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K72" s="34">
         <f>SUM(K70-J72)</f>
@@ -4188,7 +4236,7 @@
         <v>2</v>
       </c>
       <c r="F74" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G74" s="1">
         <v>0</v>
@@ -4201,7 +4249,7 @@
       </c>
       <c r="J74" s="24">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K74" s="34">
         <f>SUM(K70-J74)</f>
@@ -4231,7 +4279,7 @@
         <v>2</v>
       </c>
       <c r="F76" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G76" s="1">
         <v>3</v>
@@ -4244,7 +4292,7 @@
       </c>
       <c r="J76" s="24">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K76" s="34">
         <f>SUM(K70-J76)</f>
@@ -4274,7 +4322,7 @@
         <v>2</v>
       </c>
       <c r="F78" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G78" s="1">
         <v>3</v>
@@ -4287,7 +4335,7 @@
       </c>
       <c r="J78" s="24">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K78" s="34">
         <f>SUM(K70-J78)</f>
@@ -4341,7 +4389,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G81" s="1">
         <v>3</v>
@@ -4354,7 +4402,7 @@
       </c>
       <c r="J81" s="24">
         <f t="shared" ref="J81:J92" si="5">SUM(E81+F81+G81+H81+I81)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K81" s="34">
         <f>SUM(K70-J81)</f>
@@ -4386,7 +4434,7 @@
         <v>2</v>
       </c>
       <c r="F83" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G83" s="1">
         <v>3</v>
@@ -4399,7 +4447,7 @@
       </c>
       <c r="J83" s="24">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K83" s="34">
         <f>SUM(K70-J83)</f>
@@ -4429,7 +4477,7 @@
         <v>2</v>
       </c>
       <c r="F85" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G85" s="1">
         <v>3</v>
@@ -4442,7 +4490,7 @@
       </c>
       <c r="J85" s="24">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K85" s="34">
         <f>SUM(K70-J85)</f>
@@ -4472,7 +4520,7 @@
         <v>2</v>
       </c>
       <c r="F87" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G87" s="1">
         <v>3</v>
@@ -4485,7 +4533,7 @@
       </c>
       <c r="J87" s="24">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K87" s="34">
         <f>SUM(K70-J87)</f>
@@ -4515,7 +4563,7 @@
         <v>2</v>
       </c>
       <c r="F89" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G89" s="1">
         <v>3</v>
@@ -4528,7 +4576,7 @@
       </c>
       <c r="J89" s="24">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K89" s="34">
         <f>SUM(K70-J89)</f>
@@ -4558,7 +4606,7 @@
         <v>2</v>
       </c>
       <c r="F91" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G91" s="1">
         <v>3</v>
@@ -4571,7 +4619,7 @@
       </c>
       <c r="J91" s="24">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K91" s="34">
         <f>SUM(K70-J91)</f>
@@ -4585,11 +4633,13 @@
       <c r="E92" s="40"/>
       <c r="F92" s="40"/>
       <c r="G92" s="40"/>
-      <c r="H92" s="40"/>
+      <c r="H92" s="40">
+        <v>1</v>
+      </c>
       <c r="I92" s="41"/>
       <c r="J92" s="42">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K92" s="43"/>
     </row>
@@ -4616,7 +4666,7 @@
         <v>20</v>
       </c>
       <c r="K94" s="30">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="4:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4651,38 +4701,40 @@
         <v>0</v>
       </c>
       <c r="F96" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G96" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H96" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I96" s="20">
         <v>0</v>
       </c>
       <c r="J96" s="24">
         <f t="shared" ref="J96:J103" si="6">SUM(E96+F96+G96+H96+I96)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K96" s="34">
         <f>SUM(K94-J96)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D97" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E97" s="5"/>
+      <c r="E97" s="5">
+        <v>2</v>
+      </c>
       <c r="F97" s="5"/>
       <c r="G97" s="5"/>
       <c r="H97" s="5"/>
       <c r="I97" s="21"/>
       <c r="J97" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K97" s="36"/>
     </row>
@@ -4691,23 +4743,23 @@
         <v>7</v>
       </c>
       <c r="E98" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F98" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G98" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H98" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I98" s="20">
         <v>0</v>
       </c>
       <c r="J98" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K98" s="34">
         <f>SUM(K94-J98)</f>
@@ -4734,23 +4786,23 @@
         <v>8</v>
       </c>
       <c r="E100" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F100" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G100" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H100" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I100" s="20">
         <v>0</v>
       </c>
       <c r="J100" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K100" s="34">
         <f>SUM(K94-J100)</f>
@@ -4777,23 +4829,23 @@
         <v>5</v>
       </c>
       <c r="E102" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F102" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G102" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H102" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I102" s="20">
         <v>0</v>
       </c>
       <c r="J102" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K102" s="34">
         <f>SUM(K94-J102)</f>
@@ -4844,13 +4896,13 @@
         <v>11</v>
       </c>
       <c r="E105" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F105" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G105" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H105" s="1">
         <v>0</v>
@@ -4860,11 +4912,11 @@
       </c>
       <c r="J105" s="24">
         <f t="shared" ref="J105:J116" si="7">SUM(E105+F105+G105+H105+I105)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K105" s="34">
         <f>SUM(K94-J105)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4887,23 +4939,23 @@
         <v>12</v>
       </c>
       <c r="E107" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F107" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G107" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H107" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I107" s="20">
         <v>0</v>
       </c>
       <c r="J107" s="24">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K107" s="34">
         <f>SUM(K94-J107)</f>
@@ -4930,23 +4982,23 @@
         <v>13</v>
       </c>
       <c r="E109" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F109" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G109" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H109" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I109" s="20">
         <v>0</v>
       </c>
       <c r="J109" s="24">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K109" s="34">
         <f>SUM(K94-J109)</f>
@@ -4973,13 +5025,13 @@
         <v>26</v>
       </c>
       <c r="E111" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F111" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G111" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H111" s="1">
         <v>0</v>
@@ -4989,11 +5041,11 @@
       </c>
       <c r="J111" s="24">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K111" s="34">
         <f>SUM(K94-J111)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5016,23 +5068,23 @@
         <v>27</v>
       </c>
       <c r="E113" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F113" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G113" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H113" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I113" s="20">
         <v>0</v>
       </c>
       <c r="J113" s="24">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K113" s="34">
         <f>SUM(K94-J113)</f>
@@ -5059,23 +5111,23 @@
         <v>28</v>
       </c>
       <c r="E115" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F115" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G115" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H115" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I115" s="20">
         <v>0</v>
       </c>
       <c r="J115" s="24">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K115" s="34">
         <f>SUM(K94-J115)</f>
@@ -5089,11 +5141,13 @@
       <c r="E116" s="40"/>
       <c r="F116" s="40"/>
       <c r="G116" s="40"/>
-      <c r="H116" s="40"/>
+      <c r="H116" s="40">
+        <v>1</v>
+      </c>
       <c r="I116" s="41"/>
       <c r="J116" s="42">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K116" s="43"/>
     </row>

</xml_diff>